<commit_message>
Made optimization algorithm more 'realistic'
</commit_message>
<xml_diff>
--- a/Docs/tabu_results.xlsx
+++ b/Docs/tabu_results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FYDP\FYDPOptimizerBenchmark\FYDPOptimizerBenchmark\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FYDP\JamBot\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -731,61 +731,61 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>101.777</c:v>
+                  <c:v>0.41322999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>108.64700000000001</c:v>
+                  <c:v>0.38508799999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>110.286</c:v>
+                  <c:v>0.41073700000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>106.349</c:v>
+                  <c:v>0.38763500000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>110.07599999999999</c:v>
+                  <c:v>0.37880399999999997</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>108.827</c:v>
+                  <c:v>0.41026099999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>117.693</c:v>
+                  <c:v>0.38739600000000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>110.574</c:v>
+                  <c:v>0.40434199999999998</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>115.63500000000001</c:v>
+                  <c:v>0.37380400000000003</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>112.044</c:v>
+                  <c:v>0.404806</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>112.426</c:v>
+                  <c:v>0.39629999999999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>115.413</c:v>
+                  <c:v>0.38711499999999999</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>118.039</c:v>
+                  <c:v>0.37531599999999998</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>107.229</c:v>
+                  <c:v>0.369809</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>113.846</c:v>
+                  <c:v>0.389457</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>103.884</c:v>
+                  <c:v>0.36595299999999997</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>107.813</c:v>
+                  <c:v>0.41566199999999998</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>105.999</c:v>
+                  <c:v>0.37563600000000003</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>109.28700000000001</c:v>
+                  <c:v>0.40221000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -825,61 +825,61 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>179.21700000000001</c:v>
+                  <c:v>0.392683</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>181.41300000000001</c:v>
+                  <c:v>0.40557900000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>174.411</c:v>
+                  <c:v>0.38762600000000003</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>172.286</c:v>
+                  <c:v>0.396119</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>180.37100000000001</c:v>
+                  <c:v>0.36391899999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>178.714</c:v>
+                  <c:v>0.37741000000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>175.762</c:v>
+                  <c:v>0.35335299999999997</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>179.04</c:v>
+                  <c:v>0.39784900000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>179.77500000000001</c:v>
+                  <c:v>0.366149</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>178.44800000000001</c:v>
+                  <c:v>0.39312000000000002</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>174.548</c:v>
+                  <c:v>0.323432</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>182.179</c:v>
+                  <c:v>0.396451</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>178.279</c:v>
+                  <c:v>0.32726899999999998</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>178.54400000000001</c:v>
+                  <c:v>0.38888899999999998</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>178.232</c:v>
+                  <c:v>0.39583299999999999</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>175.51599999999999</c:v>
+                  <c:v>0.34357500000000002</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>172.43</c:v>
+                  <c:v>0.38040499999999999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>172.976</c:v>
+                  <c:v>0.42051699999999997</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>170.12100000000001</c:v>
+                  <c:v>0.39557700000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -919,61 +919,61 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>208.65799999999999</c:v>
+                  <c:v>0.407833</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>207.006</c:v>
+                  <c:v>0.38181500000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>206.76</c:v>
+                  <c:v>0.40111200000000002</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>205.98500000000001</c:v>
+                  <c:v>0.38604100000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>205.56899999999999</c:v>
+                  <c:v>0.371751</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>205.208</c:v>
+                  <c:v>0.39919300000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>204.607</c:v>
+                  <c:v>0.36396699999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>204.1</c:v>
+                  <c:v>0.36971500000000002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>204.197</c:v>
+                  <c:v>0.37907000000000002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>204.58</c:v>
+                  <c:v>0.33645900000000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>203.90299999999999</c:v>
+                  <c:v>0.389544</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>203.09399999999999</c:v>
+                  <c:v>0.41201199999999999</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>203.09100000000001</c:v>
+                  <c:v>0.375496</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>202.91</c:v>
+                  <c:v>0.39245400000000003</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>202.56800000000001</c:v>
+                  <c:v>0.41637600000000002</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>202.738</c:v>
+                  <c:v>0.43040699999999998</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>201.73500000000001</c:v>
+                  <c:v>0.37239899999999998</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>202.08600000000001</c:v>
+                  <c:v>0.38234699999999999</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>202.42099999999999</c:v>
+                  <c:v>0.408746</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -989,11 +989,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="334226720"/>
-        <c:axId val="334232880"/>
+        <c:axId val="207853520"/>
+        <c:axId val="207854080"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="334226720"/>
+        <c:axId val="207853520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1035,7 +1035,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="334232880"/>
+        <c:crossAx val="207854080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1043,7 +1043,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="334232880"/>
+        <c:axId val="207854080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1094,7 +1094,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="334226720"/>
+        <c:crossAx val="207853520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1284,61 +1284,61 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>1851.45</c:v>
+                  <c:v>4.9799799999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1887.78</c:v>
+                  <c:v>5.4392299999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2056.09</c:v>
+                  <c:v>5.3423199999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1779.71</c:v>
+                  <c:v>4.45896E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1604.35</c:v>
+                  <c:v>5.3324000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2009.7</c:v>
+                  <c:v>5.9228500000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1643.47</c:v>
+                  <c:v>3.8489500000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2002.58</c:v>
+                  <c:v>4.8006399999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2435.13</c:v>
+                  <c:v>5.2696600000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1809.38</c:v>
+                  <c:v>5.33403E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1626.52</c:v>
+                  <c:v>4.0477199999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1457.8</c:v>
+                  <c:v>5.4982700000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1679.15</c:v>
+                  <c:v>4.5572700000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2458.2800000000002</c:v>
+                  <c:v>5.2685099999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1541.89</c:v>
+                  <c:v>4.9537900000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1565.74</c:v>
+                  <c:v>4.0449699999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1940.93</c:v>
+                  <c:v>4.9705399999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1744.53</c:v>
+                  <c:v>4.2482100000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1820.5</c:v>
+                  <c:v>4.4146499999999998E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1378,61 +1378,61 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>674.86099999999999</c:v>
+                  <c:v>4.5793899999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>550.89599999999996</c:v>
+                  <c:v>5.3295000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>801.51800000000003</c:v>
+                  <c:v>5.0940699999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>808.29</c:v>
+                  <c:v>5.34923E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>575.96100000000001</c:v>
+                  <c:v>4.1907300000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>662.42600000000004</c:v>
+                  <c:v>5.2927000000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>800.75099999999998</c:v>
+                  <c:v>4.65859E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>661.79600000000005</c:v>
+                  <c:v>4.49132E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>678.85199999999998</c:v>
+                  <c:v>3.9039699999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>779.42</c:v>
+                  <c:v>4.88561E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>913.50900000000001</c:v>
+                  <c:v>4.33493E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>602.91899999999998</c:v>
+                  <c:v>4.2466999999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>839.55399999999997</c:v>
+                  <c:v>3.4722200000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>754.14099999999996</c:v>
+                  <c:v>4.8196299999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>727.16200000000003</c:v>
+                  <c:v>5.2347999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>663.524</c:v>
+                  <c:v>4.8846399999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>762.31100000000004</c:v>
+                  <c:v>4.8449800000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>751.30200000000002</c:v>
+                  <c:v>5.3605699999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>756.82500000000005</c:v>
+                  <c:v>5.21673E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1472,61 +1472,61 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>2.6262699999999999</c:v>
+                  <c:v>5.4211200000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.8927899999999998</c:v>
+                  <c:v>4.94951E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.5964799999999997</c:v>
+                  <c:v>5.2831500000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>13.7227</c:v>
+                  <c:v>5.1303799999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>14.6547</c:v>
+                  <c:v>5.2113800000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>10.7919</c:v>
+                  <c:v>4.6865400000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>17.158799999999999</c:v>
+                  <c:v>4.7343200000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>18.426200000000001</c:v>
+                  <c:v>4.4137999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>14.172499999999999</c:v>
+                  <c:v>4.5892299999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>14.708399999999999</c:v>
+                  <c:v>5.0840999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>22.7133</c:v>
+                  <c:v>4.8796300000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>22.4863</c:v>
+                  <c:v>4.8807900000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>17.845199999999998</c:v>
+                  <c:v>4.4103000000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>28.591200000000001</c:v>
+                  <c:v>5.5421900000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>21.029699999999998</c:v>
+                  <c:v>4.8130100000000002E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>18.682300000000001</c:v>
+                  <c:v>4.9035799999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>21.491800000000001</c:v>
+                  <c:v>5.2101799999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>20.912099999999999</c:v>
+                  <c:v>4.6669500000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>17.221</c:v>
+                  <c:v>5.9023100000000002E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1542,11 +1542,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="341519456"/>
-        <c:axId val="341514416"/>
+        <c:axId val="207858000"/>
+        <c:axId val="207858560"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="341519456"/>
+        <c:axId val="207858000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1588,7 +1588,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="341514416"/>
+        <c:crossAx val="207858560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1596,7 +1596,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="341514416"/>
+        <c:axId val="207858560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1647,7 +1647,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="341519456"/>
+        <c:crossAx val="207858000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1837,61 +1837,61 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>0.12</c:v>
+                  <c:v>1.28</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.14000000000000001</c:v>
+                  <c:v>1.3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.12</c:v>
+                  <c:v>1.22</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.12</c:v>
+                  <c:v>1.25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.11</c:v>
+                  <c:v>1.22</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.0000000000000007E-2</c:v>
+                  <c:v>1.28</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.1</c:v>
+                  <c:v>1.21</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.13</c:v>
+                  <c:v>1.32</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.1</c:v>
+                  <c:v>1.22</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.1</c:v>
+                  <c:v>1.25</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.1</c:v>
+                  <c:v>1.22</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.11</c:v>
+                  <c:v>1.22</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.11</c:v>
+                  <c:v>1.18</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.1</c:v>
+                  <c:v>1.1399999999999999</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.16</c:v>
+                  <c:v>1.2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.1</c:v>
+                  <c:v>1.25</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.09</c:v>
+                  <c:v>1.25</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.09</c:v>
+                  <c:v>1.19</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.09</c:v>
+                  <c:v>1.24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1931,61 +1931,61 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>0.92</c:v>
+                  <c:v>12.16</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.95</c:v>
+                  <c:v>11.95</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>12.16</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.91</c:v>
+                  <c:v>12.09</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.06</c:v>
+                  <c:v>12.15</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.06</c:v>
+                  <c:v>12.03</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.02</c:v>
+                  <c:v>12.2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.01</c:v>
+                  <c:v>12.01</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.1399999999999999</c:v>
+                  <c:v>12.02</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.06</c:v>
+                  <c:v>11.8</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.08</c:v>
+                  <c:v>11.81</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1.04</c:v>
+                  <c:v>11.75</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1.08</c:v>
+                  <c:v>11.94</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.96</c:v>
+                  <c:v>11.73</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1</c:v>
+                  <c:v>11.87</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1.21</c:v>
+                  <c:v>11.8</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1.05</c:v>
+                  <c:v>12.01</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.05</c:v>
+                  <c:v>11.8</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.01</c:v>
+                  <c:v>11.83</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2025,61 +2025,61 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>8.3800000000000008</c:v>
+                  <c:v>117.49</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.25</c:v>
+                  <c:v>121.01</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10.06</c:v>
+                  <c:v>119.22</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11.21</c:v>
+                  <c:v>131.32</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11.45</c:v>
+                  <c:v>122.46</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12.06</c:v>
+                  <c:v>128.06</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12</c:v>
+                  <c:v>120.69</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>12.18</c:v>
+                  <c:v>126.72</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>12.89</c:v>
+                  <c:v>120.54</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>13.48</c:v>
+                  <c:v>117.75</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>13.51</c:v>
+                  <c:v>115.6</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>13.37</c:v>
+                  <c:v>118.07</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>14.41</c:v>
+                  <c:v>117.65</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>15.09</c:v>
+                  <c:v>121.25</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>14.26</c:v>
+                  <c:v>125.99</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>14.52</c:v>
+                  <c:v>118.95</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>15.02</c:v>
+                  <c:v>118.51</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>15.1</c:v>
+                  <c:v>118.67</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>16.14</c:v>
+                  <c:v>120.58</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2095,11 +2095,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="342073792"/>
-        <c:axId val="342084432"/>
+        <c:axId val="245642464"/>
+        <c:axId val="245643024"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="342073792"/>
+        <c:axId val="245642464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2141,7 +2141,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="342084432"/>
+        <c:crossAx val="245643024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2149,7 +2149,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="342084432"/>
+        <c:axId val="245643024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2200,7 +2200,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="342073792"/>
+        <c:crossAx val="245642464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2390,61 +2390,61 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>190.81200000000001</c:v>
+                  <c:v>0.989672</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>203.92500000000001</c:v>
+                  <c:v>0.97313700000000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>196.65899999999999</c:v>
+                  <c:v>0.98524199999999995</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>209.93299999999999</c:v>
+                  <c:v>0.920242</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>194.364</c:v>
+                  <c:v>0.85992500000000005</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>203.06</c:v>
+                  <c:v>0.94246399999999997</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>198.32400000000001</c:v>
+                  <c:v>0.86858900000000006</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>201.98500000000001</c:v>
+                  <c:v>0.83135300000000001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>206.55600000000001</c:v>
+                  <c:v>0.89802000000000004</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>205.56299999999999</c:v>
+                  <c:v>0.91303400000000001</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>193.90199999999999</c:v>
+                  <c:v>0.88135300000000005</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>205.88900000000001</c:v>
+                  <c:v>0.87135300000000004</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>200.03899999999999</c:v>
+                  <c:v>0.84413099999999996</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>196.82900000000001</c:v>
+                  <c:v>0.86563900000000005</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>188.30799999999999</c:v>
+                  <c:v>0.893258</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>192.05199999999999</c:v>
+                  <c:v>0.86468599999999995</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>197.791</c:v>
+                  <c:v>0.85194899999999996</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>207.36</c:v>
+                  <c:v>0.93135299999999999</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>199.208</c:v>
+                  <c:v>0.85992500000000005</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2484,61 +2484,61 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>210</c:v>
+                  <c:v>0.88341800000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>209.495</c:v>
+                  <c:v>0.893258</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>210</c:v>
+                  <c:v>0.86526899999999995</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>210</c:v>
+                  <c:v>0.89802000000000004</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>210</c:v>
+                  <c:v>0.81761200000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>210</c:v>
+                  <c:v>0.88135300000000005</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>209.44900000000001</c:v>
+                  <c:v>0.85633899999999996</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>208.90899999999999</c:v>
+                  <c:v>0.87933799999999995</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>210</c:v>
+                  <c:v>0.831036</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>210</c:v>
+                  <c:v>0.91913100000000003</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>210</c:v>
+                  <c:v>0.87936199999999998</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>209.715</c:v>
+                  <c:v>0.88135300000000005</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>208.953</c:v>
+                  <c:v>0.86996399999999996</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>210</c:v>
+                  <c:v>1.03135</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>210</c:v>
+                  <c:v>0.90226200000000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>209.22900000000001</c:v>
+                  <c:v>0.81824399999999997</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>210</c:v>
+                  <c:v>0.83730599999999999</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>209.65899999999999</c:v>
+                  <c:v>0.95867500000000005</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>209.828</c:v>
+                  <c:v>1.01267</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2578,61 +2578,61 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>210</c:v>
+                  <c:v>0.96306000000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>210</c:v>
+                  <c:v>0.86468599999999995</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>210</c:v>
+                  <c:v>0.91107199999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>210</c:v>
+                  <c:v>1.00814</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>210</c:v>
+                  <c:v>0.88690899999999995</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>210</c:v>
+                  <c:v>0.79801999999999995</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>210</c:v>
+                  <c:v>0.85635300000000003</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>210</c:v>
+                  <c:v>0.83546299999999996</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>210</c:v>
+                  <c:v>0.84770199999999996</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>210</c:v>
+                  <c:v>0.88817999999999997</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>209.83199999999999</c:v>
+                  <c:v>0.96202799999999999</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>210</c:v>
+                  <c:v>0.84602900000000003</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>210</c:v>
+                  <c:v>0.86468599999999995</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>210</c:v>
+                  <c:v>0.88642900000000002</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>209.90799999999999</c:v>
+                  <c:v>0.863537</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>210</c:v>
+                  <c:v>0.93751799999999996</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>209.49199999999999</c:v>
+                  <c:v>0.86468599999999995</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>210</c:v>
+                  <c:v>0.92975300000000005</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>209.76900000000001</c:v>
+                  <c:v>0.94246399999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2648,11 +2648,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="329328896"/>
-        <c:axId val="329328336"/>
+        <c:axId val="245646944"/>
+        <c:axId val="245647504"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="329328896"/>
+        <c:axId val="245646944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2694,7 +2694,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="329328336"/>
+        <c:crossAx val="245647504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2702,7 +2702,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="329328336"/>
+        <c:axId val="245647504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2753,7 +2753,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="329328896"/>
+        <c:crossAx val="245646944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5448,8 +5448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="U5" sqref="U5"/>
+    <sheetView tabSelected="1" topLeftCell="H13" workbookViewId="0">
+      <selection activeCell="U23" sqref="U23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5482,16 +5482,16 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>101.777</v>
+        <v>0.41322999999999999</v>
       </c>
       <c r="D2">
-        <v>190.81200000000001</v>
+        <v>0.989672</v>
       </c>
       <c r="E2">
-        <v>1851.45</v>
+        <v>4.9799799999999998E-2</v>
       </c>
       <c r="F2">
-        <v>0.12</v>
+        <v>1.28</v>
       </c>
       <c r="H2" t="s">
         <v>0</v>
@@ -5514,28 +5514,28 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>108.64700000000001</v>
+        <v>0.38508799999999999</v>
       </c>
       <c r="D3">
-        <v>203.92500000000001</v>
+        <v>0.97313700000000003</v>
       </c>
       <c r="E3">
-        <v>1887.78</v>
+        <v>5.4392299999999998E-2</v>
       </c>
       <c r="F3">
-        <v>0.14000000000000001</v>
+        <v>1.3</v>
       </c>
       <c r="H3">
         <v>1</v>
       </c>
       <c r="I3">
-        <v>101.777</v>
+        <v>0.41322999999999999</v>
       </c>
       <c r="J3">
-        <v>179.21700000000001</v>
+        <v>0.392683</v>
       </c>
       <c r="K3">
-        <v>208.65799999999999</v>
+        <v>0.407833</v>
       </c>
       <c r="U3" t="s">
         <v>18</v>
@@ -5549,28 +5549,28 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>110.286</v>
+        <v>0.41073700000000002</v>
       </c>
       <c r="D4">
-        <v>196.65899999999999</v>
+        <v>0.98524199999999995</v>
       </c>
       <c r="E4">
-        <v>2056.09</v>
+        <v>5.3423199999999997E-2</v>
       </c>
       <c r="F4">
-        <v>0.12</v>
+        <v>1.22</v>
       </c>
       <c r="H4">
         <v>2</v>
       </c>
       <c r="I4">
-        <v>108.64700000000001</v>
+        <v>0.38508799999999999</v>
       </c>
       <c r="J4">
-        <v>181.41300000000001</v>
+        <v>0.40557900000000002</v>
       </c>
       <c r="K4">
-        <v>207.006</v>
+        <v>0.38181500000000002</v>
       </c>
       <c r="U4" t="s">
         <v>19</v>
@@ -5584,28 +5584,28 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>106.349</v>
+        <v>0.38763500000000001</v>
       </c>
       <c r="D5">
-        <v>209.93299999999999</v>
+        <v>0.920242</v>
       </c>
       <c r="E5">
-        <v>1779.71</v>
+        <v>4.45896E-2</v>
       </c>
       <c r="F5">
-        <v>0.12</v>
+        <v>1.25</v>
       </c>
       <c r="H5">
         <v>3</v>
       </c>
       <c r="I5">
-        <v>110.286</v>
+        <v>0.41073700000000002</v>
       </c>
       <c r="J5">
-        <v>174.411</v>
+        <v>0.38762600000000003</v>
       </c>
       <c r="K5">
-        <v>206.76</v>
+        <v>0.40111200000000002</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
@@ -5616,28 +5616,28 @@
         <v>1</v>
       </c>
       <c r="C6">
-        <v>110.07599999999999</v>
+        <v>0.37880399999999997</v>
       </c>
       <c r="D6">
-        <v>194.364</v>
+        <v>0.85992500000000005</v>
       </c>
       <c r="E6">
-        <v>1604.35</v>
+        <v>5.3324000000000003E-2</v>
       </c>
       <c r="F6">
-        <v>0.11</v>
+        <v>1.22</v>
       </c>
       <c r="H6">
         <v>4</v>
       </c>
       <c r="I6">
-        <v>106.349</v>
+        <v>0.38763500000000001</v>
       </c>
       <c r="J6">
-        <v>172.286</v>
+        <v>0.396119</v>
       </c>
       <c r="K6">
-        <v>205.98500000000001</v>
+        <v>0.38604100000000002</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
@@ -5648,28 +5648,28 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>108.827</v>
+        <v>0.41026099999999999</v>
       </c>
       <c r="D7">
-        <v>203.06</v>
+        <v>0.94246399999999997</v>
       </c>
       <c r="E7">
-        <v>2009.7</v>
+        <v>5.9228500000000003E-2</v>
       </c>
       <c r="F7">
-        <v>7.0000000000000007E-2</v>
+        <v>1.28</v>
       </c>
       <c r="H7">
         <v>5</v>
       </c>
       <c r="I7">
-        <v>110.07599999999999</v>
+        <v>0.37880399999999997</v>
       </c>
       <c r="J7">
-        <v>180.37100000000001</v>
+        <v>0.36391899999999999</v>
       </c>
       <c r="K7">
-        <v>205.56899999999999</v>
+        <v>0.371751</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
@@ -5680,28 +5680,28 @@
         <v>1</v>
       </c>
       <c r="C8">
-        <v>117.693</v>
+        <v>0.38739600000000002</v>
       </c>
       <c r="D8">
-        <v>198.32400000000001</v>
+        <v>0.86858900000000006</v>
       </c>
       <c r="E8">
-        <v>1643.47</v>
+        <v>3.8489500000000003E-2</v>
       </c>
       <c r="F8">
-        <v>0.1</v>
+        <v>1.21</v>
       </c>
       <c r="H8">
         <v>6</v>
       </c>
       <c r="I8">
-        <v>108.827</v>
+        <v>0.41026099999999999</v>
       </c>
       <c r="J8">
-        <v>178.714</v>
+        <v>0.37741000000000002</v>
       </c>
       <c r="K8">
-        <v>205.208</v>
+        <v>0.39919300000000002</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
@@ -5712,28 +5712,28 @@
         <v>1</v>
       </c>
       <c r="C9">
-        <v>110.574</v>
+        <v>0.40434199999999998</v>
       </c>
       <c r="D9">
-        <v>201.98500000000001</v>
+        <v>0.83135300000000001</v>
       </c>
       <c r="E9">
-        <v>2002.58</v>
+        <v>4.8006399999999998E-2</v>
       </c>
       <c r="F9">
-        <v>0.13</v>
+        <v>1.32</v>
       </c>
       <c r="H9">
         <v>7</v>
       </c>
       <c r="I9">
-        <v>117.693</v>
+        <v>0.38739600000000002</v>
       </c>
       <c r="J9">
-        <v>175.762</v>
+        <v>0.35335299999999997</v>
       </c>
       <c r="K9">
-        <v>204.607</v>
+        <v>0.36396699999999998</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
@@ -5744,28 +5744,28 @@
         <v>1</v>
       </c>
       <c r="C10">
-        <v>115.63500000000001</v>
+        <v>0.37380400000000003</v>
       </c>
       <c r="D10">
-        <v>206.55600000000001</v>
+        <v>0.89802000000000004</v>
       </c>
       <c r="E10">
-        <v>2435.13</v>
+        <v>5.2696600000000003E-2</v>
       </c>
       <c r="F10">
-        <v>0.1</v>
+        <v>1.22</v>
       </c>
       <c r="H10">
         <v>8</v>
       </c>
       <c r="I10">
-        <v>110.574</v>
+        <v>0.40434199999999998</v>
       </c>
       <c r="J10">
-        <v>179.04</v>
+        <v>0.39784900000000001</v>
       </c>
       <c r="K10">
-        <v>204.1</v>
+        <v>0.36971500000000002</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
@@ -5776,28 +5776,28 @@
         <v>1</v>
       </c>
       <c r="C11">
-        <v>112.044</v>
+        <v>0.404806</v>
       </c>
       <c r="D11">
-        <v>205.56299999999999</v>
+        <v>0.91303400000000001</v>
       </c>
       <c r="E11">
-        <v>1809.38</v>
+        <v>5.33403E-2</v>
       </c>
       <c r="F11">
-        <v>0.1</v>
+        <v>1.25</v>
       </c>
       <c r="H11">
         <v>9</v>
       </c>
       <c r="I11">
-        <v>115.63500000000001</v>
+        <v>0.37380400000000003</v>
       </c>
       <c r="J11">
-        <v>179.77500000000001</v>
+        <v>0.366149</v>
       </c>
       <c r="K11">
-        <v>204.197</v>
+        <v>0.37907000000000002</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
@@ -5808,28 +5808,28 @@
         <v>1</v>
       </c>
       <c r="C12">
-        <v>112.426</v>
+        <v>0.39629999999999999</v>
       </c>
       <c r="D12">
-        <v>193.90199999999999</v>
+        <v>0.88135300000000005</v>
       </c>
       <c r="E12">
-        <v>1626.52</v>
+        <v>4.0477199999999998E-2</v>
       </c>
       <c r="F12">
-        <v>0.1</v>
+        <v>1.22</v>
       </c>
       <c r="H12">
         <v>10</v>
       </c>
       <c r="I12">
-        <v>112.044</v>
+        <v>0.404806</v>
       </c>
       <c r="J12">
-        <v>178.44800000000001</v>
+        <v>0.39312000000000002</v>
       </c>
       <c r="K12">
-        <v>204.58</v>
+        <v>0.33645900000000001</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
@@ -5840,28 +5840,28 @@
         <v>1</v>
       </c>
       <c r="C13">
-        <v>115.413</v>
+        <v>0.38711499999999999</v>
       </c>
       <c r="D13">
-        <v>205.88900000000001</v>
+        <v>0.87135300000000004</v>
       </c>
       <c r="E13">
-        <v>1457.8</v>
+        <v>5.4982700000000002E-2</v>
       </c>
       <c r="F13">
-        <v>0.11</v>
+        <v>1.22</v>
       </c>
       <c r="H13">
         <v>11</v>
       </c>
       <c r="I13">
-        <v>112.426</v>
+        <v>0.39629999999999999</v>
       </c>
       <c r="J13">
-        <v>174.548</v>
+        <v>0.323432</v>
       </c>
       <c r="K13">
-        <v>203.90299999999999</v>
+        <v>0.389544</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
@@ -5872,28 +5872,28 @@
         <v>1</v>
       </c>
       <c r="C14">
-        <v>118.039</v>
+        <v>0.37531599999999998</v>
       </c>
       <c r="D14">
-        <v>200.03899999999999</v>
+        <v>0.84413099999999996</v>
       </c>
       <c r="E14">
-        <v>1679.15</v>
+        <v>4.5572700000000001E-2</v>
       </c>
       <c r="F14">
-        <v>0.11</v>
+        <v>1.18</v>
       </c>
       <c r="H14">
         <v>12</v>
       </c>
       <c r="I14">
-        <v>115.413</v>
+        <v>0.38711499999999999</v>
       </c>
       <c r="J14">
-        <v>182.179</v>
+        <v>0.396451</v>
       </c>
       <c r="K14">
-        <v>203.09399999999999</v>
+        <v>0.41201199999999999</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
@@ -5904,28 +5904,28 @@
         <v>1</v>
       </c>
       <c r="C15">
-        <v>107.229</v>
+        <v>0.369809</v>
       </c>
       <c r="D15">
-        <v>196.82900000000001</v>
+        <v>0.86563900000000005</v>
       </c>
       <c r="E15">
-        <v>2458.2800000000002</v>
+        <v>5.2685099999999999E-2</v>
       </c>
       <c r="F15">
-        <v>0.1</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="H15">
         <v>13</v>
       </c>
       <c r="I15">
-        <v>118.039</v>
+        <v>0.37531599999999998</v>
       </c>
       <c r="J15">
-        <v>178.279</v>
+        <v>0.32726899999999998</v>
       </c>
       <c r="K15">
-        <v>203.09100000000001</v>
+        <v>0.375496</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
@@ -5936,28 +5936,28 @@
         <v>1</v>
       </c>
       <c r="C16">
-        <v>113.846</v>
+        <v>0.389457</v>
       </c>
       <c r="D16">
-        <v>188.30799999999999</v>
+        <v>0.893258</v>
       </c>
       <c r="E16">
-        <v>1541.89</v>
+        <v>4.9537900000000003E-2</v>
       </c>
       <c r="F16">
-        <v>0.16</v>
+        <v>1.2</v>
       </c>
       <c r="H16">
         <v>14</v>
       </c>
       <c r="I16">
-        <v>107.229</v>
+        <v>0.369809</v>
       </c>
       <c r="J16">
-        <v>178.54400000000001</v>
+        <v>0.38888899999999998</v>
       </c>
       <c r="K16">
-        <v>202.91</v>
+        <v>0.39245400000000003</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -5968,28 +5968,28 @@
         <v>1</v>
       </c>
       <c r="C17">
-        <v>103.884</v>
+        <v>0.36595299999999997</v>
       </c>
       <c r="D17">
-        <v>192.05199999999999</v>
+        <v>0.86468599999999995</v>
       </c>
       <c r="E17">
-        <v>1565.74</v>
+        <v>4.0449699999999998E-2</v>
       </c>
       <c r="F17">
-        <v>0.1</v>
+        <v>1.25</v>
       </c>
       <c r="H17">
         <v>15</v>
       </c>
       <c r="I17">
-        <v>113.846</v>
+        <v>0.389457</v>
       </c>
       <c r="J17">
-        <v>178.232</v>
+        <v>0.39583299999999999</v>
       </c>
       <c r="K17">
-        <v>202.56800000000001</v>
+        <v>0.41637600000000002</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -6000,28 +6000,28 @@
         <v>1</v>
       </c>
       <c r="C18">
-        <v>107.813</v>
+        <v>0.41566199999999998</v>
       </c>
       <c r="D18">
-        <v>197.791</v>
+        <v>0.85194899999999996</v>
       </c>
       <c r="E18">
-        <v>1940.93</v>
+        <v>4.9705399999999997E-2</v>
       </c>
       <c r="F18">
-        <v>0.09</v>
+        <v>1.25</v>
       </c>
       <c r="H18">
         <v>16</v>
       </c>
       <c r="I18">
-        <v>103.884</v>
+        <v>0.36595299999999997</v>
       </c>
       <c r="J18">
-        <v>175.51599999999999</v>
+        <v>0.34357500000000002</v>
       </c>
       <c r="K18">
-        <v>202.738</v>
+        <v>0.43040699999999998</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -6032,28 +6032,28 @@
         <v>1</v>
       </c>
       <c r="C19">
-        <v>105.999</v>
+        <v>0.37563600000000003</v>
       </c>
       <c r="D19">
-        <v>207.36</v>
+        <v>0.93135299999999999</v>
       </c>
       <c r="E19">
-        <v>1744.53</v>
+        <v>4.2482100000000002E-2</v>
       </c>
       <c r="F19">
-        <v>0.09</v>
+        <v>1.19</v>
       </c>
       <c r="H19">
         <v>17</v>
       </c>
       <c r="I19">
-        <v>107.813</v>
+        <v>0.41566199999999998</v>
       </c>
       <c r="J19">
-        <v>172.43</v>
+        <v>0.38040499999999999</v>
       </c>
       <c r="K19">
-        <v>201.73500000000001</v>
+        <v>0.37239899999999998</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -6064,28 +6064,28 @@
         <v>1</v>
       </c>
       <c r="C20">
-        <v>109.28700000000001</v>
+        <v>0.40221000000000001</v>
       </c>
       <c r="D20">
-        <v>199.208</v>
+        <v>0.85992500000000005</v>
       </c>
       <c r="E20">
-        <v>1820.5</v>
+        <v>4.4146499999999998E-2</v>
       </c>
       <c r="F20">
-        <v>0.09</v>
+        <v>1.24</v>
       </c>
       <c r="H20">
         <v>18</v>
       </c>
       <c r="I20">
-        <v>105.999</v>
+        <v>0.37563600000000003</v>
       </c>
       <c r="J20">
-        <v>172.976</v>
+        <v>0.42051699999999997</v>
       </c>
       <c r="K20">
-        <v>202.08600000000001</v>
+        <v>0.38234699999999999</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -6096,28 +6096,28 @@
         <v>10</v>
       </c>
       <c r="C21">
-        <v>179.21700000000001</v>
+        <v>0.392683</v>
       </c>
       <c r="D21">
-        <v>210</v>
+        <v>0.88341800000000004</v>
       </c>
       <c r="E21">
-        <v>674.86099999999999</v>
+        <v>4.5793899999999998E-2</v>
       </c>
       <c r="F21">
-        <v>0.92</v>
+        <v>12.16</v>
       </c>
       <c r="H21">
         <v>19</v>
       </c>
       <c r="I21">
-        <v>109.28700000000001</v>
+        <v>0.40221000000000001</v>
       </c>
       <c r="J21">
-        <v>170.12100000000001</v>
+        <v>0.39557700000000001</v>
       </c>
       <c r="K21">
-        <v>202.42099999999999</v>
+        <v>0.408746</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -6128,16 +6128,16 @@
         <v>10</v>
       </c>
       <c r="C22">
-        <v>181.41300000000001</v>
+        <v>0.40557900000000002</v>
       </c>
       <c r="D22">
-        <v>209.495</v>
+        <v>0.893258</v>
       </c>
       <c r="E22">
-        <v>550.89599999999996</v>
+        <v>5.3295000000000002E-2</v>
       </c>
       <c r="F22">
-        <v>0.95</v>
+        <v>11.95</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -6148,16 +6148,16 @@
         <v>10</v>
       </c>
       <c r="C23">
-        <v>174.411</v>
+        <v>0.38762600000000003</v>
       </c>
       <c r="D23">
-        <v>210</v>
+        <v>0.86526899999999995</v>
       </c>
       <c r="E23">
-        <v>801.51800000000003</v>
+        <v>5.0940699999999998E-2</v>
       </c>
       <c r="F23">
-        <v>1</v>
+        <v>12.16</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -6168,16 +6168,16 @@
         <v>10</v>
       </c>
       <c r="C24">
-        <v>172.286</v>
+        <v>0.396119</v>
       </c>
       <c r="D24">
-        <v>210</v>
+        <v>0.89802000000000004</v>
       </c>
       <c r="E24">
-        <v>808.29</v>
+        <v>5.34923E-2</v>
       </c>
       <c r="F24">
-        <v>0.91</v>
+        <v>12.09</v>
       </c>
       <c r="H24" t="s">
         <v>0</v>
@@ -6200,28 +6200,28 @@
         <v>10</v>
       </c>
       <c r="C25">
-        <v>180.37100000000001</v>
+        <v>0.36391899999999999</v>
       </c>
       <c r="D25">
-        <v>210</v>
+        <v>0.81761200000000001</v>
       </c>
       <c r="E25">
-        <v>575.96100000000001</v>
+        <v>4.1907300000000001E-2</v>
       </c>
       <c r="F25">
-        <v>1.06</v>
+        <v>12.15</v>
       </c>
       <c r="H25">
         <v>1</v>
       </c>
       <c r="I25">
-        <v>1851.45</v>
+        <v>4.9799799999999998E-2</v>
       </c>
       <c r="J25">
-        <v>674.86099999999999</v>
+        <v>4.5793899999999998E-2</v>
       </c>
       <c r="K25">
-        <v>2.6262699999999999</v>
+        <v>5.4211200000000001E-2</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -6232,28 +6232,28 @@
         <v>10</v>
       </c>
       <c r="C26">
-        <v>178.714</v>
+        <v>0.37741000000000002</v>
       </c>
       <c r="D26">
-        <v>210</v>
+        <v>0.88135300000000005</v>
       </c>
       <c r="E26">
-        <v>662.42600000000004</v>
+        <v>5.2927000000000002E-2</v>
       </c>
       <c r="F26">
-        <v>1.06</v>
+        <v>12.03</v>
       </c>
       <c r="H26">
         <v>2</v>
       </c>
       <c r="I26">
-        <v>1887.78</v>
+        <v>5.4392299999999998E-2</v>
       </c>
       <c r="J26">
-        <v>550.89599999999996</v>
+        <v>5.3295000000000002E-2</v>
       </c>
       <c r="K26">
-        <v>8.8927899999999998</v>
+        <v>4.94951E-2</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -6264,28 +6264,28 @@
         <v>10</v>
       </c>
       <c r="C27">
-        <v>175.762</v>
+        <v>0.35335299999999997</v>
       </c>
       <c r="D27">
-        <v>209.44900000000001</v>
+        <v>0.85633899999999996</v>
       </c>
       <c r="E27">
-        <v>800.75099999999998</v>
+        <v>4.65859E-2</v>
       </c>
       <c r="F27">
-        <v>1.02</v>
+        <v>12.2</v>
       </c>
       <c r="H27">
         <v>3</v>
       </c>
       <c r="I27">
-        <v>2056.09</v>
+        <v>5.3423199999999997E-2</v>
       </c>
       <c r="J27">
-        <v>801.51800000000003</v>
+        <v>5.0940699999999998E-2</v>
       </c>
       <c r="K27">
-        <v>7.5964799999999997</v>
+        <v>5.2831500000000003E-2</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -6296,28 +6296,28 @@
         <v>10</v>
       </c>
       <c r="C28">
-        <v>179.04</v>
+        <v>0.39784900000000001</v>
       </c>
       <c r="D28">
-        <v>208.90899999999999</v>
+        <v>0.87933799999999995</v>
       </c>
       <c r="E28">
-        <v>661.79600000000005</v>
+        <v>4.49132E-2</v>
       </c>
       <c r="F28">
-        <v>1.01</v>
+        <v>12.01</v>
       </c>
       <c r="H28">
         <v>4</v>
       </c>
       <c r="I28">
-        <v>1779.71</v>
+        <v>4.45896E-2</v>
       </c>
       <c r="J28">
-        <v>808.29</v>
+        <v>5.34923E-2</v>
       </c>
       <c r="K28">
-        <v>13.7227</v>
+        <v>5.1303799999999997E-2</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -6328,28 +6328,28 @@
         <v>10</v>
       </c>
       <c r="C29">
-        <v>179.77500000000001</v>
+        <v>0.366149</v>
       </c>
       <c r="D29">
-        <v>210</v>
+        <v>0.831036</v>
       </c>
       <c r="E29">
-        <v>678.85199999999998</v>
+        <v>3.9039699999999997E-2</v>
       </c>
       <c r="F29">
-        <v>1.1399999999999999</v>
+        <v>12.02</v>
       </c>
       <c r="H29">
         <v>5</v>
       </c>
       <c r="I29">
-        <v>1604.35</v>
+        <v>5.3324000000000003E-2</v>
       </c>
       <c r="J29">
-        <v>575.96100000000001</v>
+        <v>4.1907300000000001E-2</v>
       </c>
       <c r="K29">
-        <v>14.6547</v>
+        <v>5.2113800000000002E-2</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -6360,28 +6360,28 @@
         <v>10</v>
       </c>
       <c r="C30">
-        <v>178.44800000000001</v>
+        <v>0.39312000000000002</v>
       </c>
       <c r="D30">
-        <v>210</v>
+        <v>0.91913100000000003</v>
       </c>
       <c r="E30">
-        <v>779.42</v>
+        <v>4.88561E-2</v>
       </c>
       <c r="F30">
-        <v>1.06</v>
+        <v>11.8</v>
       </c>
       <c r="H30">
         <v>6</v>
       </c>
       <c r="I30">
-        <v>2009.7</v>
+        <v>5.9228500000000003E-2</v>
       </c>
       <c r="J30">
-        <v>662.42600000000004</v>
+        <v>5.2927000000000002E-2</v>
       </c>
       <c r="K30">
-        <v>10.7919</v>
+        <v>4.6865400000000002E-2</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -6392,28 +6392,28 @@
         <v>10</v>
       </c>
       <c r="C31">
-        <v>174.548</v>
+        <v>0.323432</v>
       </c>
       <c r="D31">
-        <v>210</v>
+        <v>0.87936199999999998</v>
       </c>
       <c r="E31">
-        <v>913.50900000000001</v>
+        <v>4.33493E-2</v>
       </c>
       <c r="F31">
-        <v>1.08</v>
+        <v>11.81</v>
       </c>
       <c r="H31">
         <v>7</v>
       </c>
       <c r="I31">
-        <v>1643.47</v>
+        <v>3.8489500000000003E-2</v>
       </c>
       <c r="J31">
-        <v>800.75099999999998</v>
+        <v>4.65859E-2</v>
       </c>
       <c r="K31">
-        <v>17.158799999999999</v>
+        <v>4.7343200000000002E-2</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -6424,28 +6424,28 @@
         <v>10</v>
       </c>
       <c r="C32">
-        <v>182.179</v>
+        <v>0.396451</v>
       </c>
       <c r="D32">
-        <v>209.715</v>
+        <v>0.88135300000000005</v>
       </c>
       <c r="E32">
-        <v>602.91899999999998</v>
+        <v>4.2466999999999998E-2</v>
       </c>
       <c r="F32">
-        <v>1.04</v>
+        <v>11.75</v>
       </c>
       <c r="H32">
         <v>8</v>
       </c>
       <c r="I32">
-        <v>2002.58</v>
+        <v>4.8006399999999998E-2</v>
       </c>
       <c r="J32">
-        <v>661.79600000000005</v>
+        <v>4.49132E-2</v>
       </c>
       <c r="K32">
-        <v>18.426200000000001</v>
+        <v>4.4137999999999997E-2</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -6456,28 +6456,28 @@
         <v>10</v>
       </c>
       <c r="C33">
-        <v>178.279</v>
+        <v>0.32726899999999998</v>
       </c>
       <c r="D33">
-        <v>208.953</v>
+        <v>0.86996399999999996</v>
       </c>
       <c r="E33">
-        <v>839.55399999999997</v>
+        <v>3.4722200000000002E-2</v>
       </c>
       <c r="F33">
-        <v>1.08</v>
+        <v>11.94</v>
       </c>
       <c r="H33">
         <v>9</v>
       </c>
       <c r="I33">
-        <v>2435.13</v>
+        <v>5.2696600000000003E-2</v>
       </c>
       <c r="J33">
-        <v>678.85199999999998</v>
+        <v>3.9039699999999997E-2</v>
       </c>
       <c r="K33">
-        <v>14.172499999999999</v>
+        <v>4.5892299999999997E-2</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
@@ -6488,28 +6488,28 @@
         <v>10</v>
       </c>
       <c r="C34">
-        <v>178.54400000000001</v>
+        <v>0.38888899999999998</v>
       </c>
       <c r="D34">
-        <v>210</v>
+        <v>1.03135</v>
       </c>
       <c r="E34">
-        <v>754.14099999999996</v>
+        <v>4.8196299999999997E-2</v>
       </c>
       <c r="F34">
-        <v>0.96</v>
+        <v>11.73</v>
       </c>
       <c r="H34">
         <v>10</v>
       </c>
       <c r="I34">
-        <v>1809.38</v>
+        <v>5.33403E-2</v>
       </c>
       <c r="J34">
-        <v>779.42</v>
+        <v>4.88561E-2</v>
       </c>
       <c r="K34">
-        <v>14.708399999999999</v>
+        <v>5.0840999999999997E-2</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -6520,28 +6520,28 @@
         <v>10</v>
       </c>
       <c r="C35">
-        <v>178.232</v>
+        <v>0.39583299999999999</v>
       </c>
       <c r="D35">
-        <v>210</v>
+        <v>0.90226200000000001</v>
       </c>
       <c r="E35">
-        <v>727.16200000000003</v>
+        <v>5.2347999999999999E-2</v>
       </c>
       <c r="F35">
-        <v>1</v>
+        <v>11.87</v>
       </c>
       <c r="H35">
         <v>11</v>
       </c>
       <c r="I35">
-        <v>1626.52</v>
+        <v>4.0477199999999998E-2</v>
       </c>
       <c r="J35">
-        <v>913.50900000000001</v>
+        <v>4.33493E-2</v>
       </c>
       <c r="K35">
-        <v>22.7133</v>
+        <v>4.8796300000000001E-2</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -6552,28 +6552,28 @@
         <v>10</v>
       </c>
       <c r="C36">
-        <v>175.51599999999999</v>
+        <v>0.34357500000000002</v>
       </c>
       <c r="D36">
-        <v>209.22900000000001</v>
+        <v>0.81824399999999997</v>
       </c>
       <c r="E36">
-        <v>663.524</v>
+        <v>4.8846399999999998E-2</v>
       </c>
       <c r="F36">
-        <v>1.21</v>
+        <v>11.8</v>
       </c>
       <c r="H36">
         <v>12</v>
       </c>
       <c r="I36">
-        <v>1457.8</v>
+        <v>5.4982700000000002E-2</v>
       </c>
       <c r="J36">
-        <v>602.91899999999998</v>
+        <v>4.2466999999999998E-2</v>
       </c>
       <c r="K36">
-        <v>22.4863</v>
+        <v>4.8807900000000001E-2</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -6584,28 +6584,28 @@
         <v>10</v>
       </c>
       <c r="C37">
-        <v>172.43</v>
+        <v>0.38040499999999999</v>
       </c>
       <c r="D37">
-        <v>210</v>
+        <v>0.83730599999999999</v>
       </c>
       <c r="E37">
-        <v>762.31100000000004</v>
+        <v>4.8449800000000001E-2</v>
       </c>
       <c r="F37">
-        <v>1.05</v>
+        <v>12.01</v>
       </c>
       <c r="H37">
         <v>13</v>
       </c>
       <c r="I37">
-        <v>1679.15</v>
+        <v>4.5572700000000001E-2</v>
       </c>
       <c r="J37">
-        <v>839.55399999999997</v>
+        <v>3.4722200000000002E-2</v>
       </c>
       <c r="K37">
-        <v>17.845199999999998</v>
+        <v>4.4103000000000003E-2</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
@@ -6616,28 +6616,28 @@
         <v>10</v>
       </c>
       <c r="C38">
-        <v>172.976</v>
+        <v>0.42051699999999997</v>
       </c>
       <c r="D38">
-        <v>209.65899999999999</v>
+        <v>0.95867500000000005</v>
       </c>
       <c r="E38">
-        <v>751.30200000000002</v>
+        <v>5.3605699999999999E-2</v>
       </c>
       <c r="F38">
-        <v>1.05</v>
+        <v>11.8</v>
       </c>
       <c r="H38">
         <v>14</v>
       </c>
       <c r="I38">
-        <v>2458.2800000000002</v>
+        <v>5.2685099999999999E-2</v>
       </c>
       <c r="J38">
-        <v>754.14099999999996</v>
+        <v>4.8196299999999997E-2</v>
       </c>
       <c r="K38">
-        <v>28.591200000000001</v>
+        <v>5.5421900000000003E-2</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -6648,28 +6648,28 @@
         <v>10</v>
       </c>
       <c r="C39">
-        <v>170.12100000000001</v>
+        <v>0.39557700000000001</v>
       </c>
       <c r="D39">
-        <v>209.828</v>
+        <v>1.01267</v>
       </c>
       <c r="E39">
-        <v>756.82500000000005</v>
+        <v>5.21673E-2</v>
       </c>
       <c r="F39">
-        <v>1.01</v>
+        <v>11.83</v>
       </c>
       <c r="H39">
         <v>15</v>
       </c>
       <c r="I39">
-        <v>1541.89</v>
+        <v>4.9537900000000003E-2</v>
       </c>
       <c r="J39">
-        <v>727.16200000000003</v>
+        <v>5.2347999999999999E-2</v>
       </c>
       <c r="K39">
-        <v>21.029699999999998</v>
+        <v>4.8130100000000002E-2</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
@@ -6680,28 +6680,28 @@
         <v>100</v>
       </c>
       <c r="C40">
-        <v>208.65799999999999</v>
+        <v>0.407833</v>
       </c>
       <c r="D40">
-        <v>210</v>
+        <v>0.96306000000000003</v>
       </c>
       <c r="E40">
-        <v>2.6262699999999999</v>
+        <v>5.4211200000000001E-2</v>
       </c>
       <c r="F40">
-        <v>8.3800000000000008</v>
+        <v>117.49</v>
       </c>
       <c r="H40">
         <v>16</v>
       </c>
       <c r="I40">
-        <v>1565.74</v>
+        <v>4.0449699999999998E-2</v>
       </c>
       <c r="J40">
-        <v>663.524</v>
+        <v>4.8846399999999998E-2</v>
       </c>
       <c r="K40">
-        <v>18.682300000000001</v>
+        <v>4.9035799999999997E-2</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
@@ -6712,28 +6712,28 @@
         <v>100</v>
       </c>
       <c r="C41">
-        <v>207.006</v>
+        <v>0.38181500000000002</v>
       </c>
       <c r="D41">
-        <v>210</v>
+        <v>0.86468599999999995</v>
       </c>
       <c r="E41">
-        <v>8.8927899999999998</v>
+        <v>4.94951E-2</v>
       </c>
       <c r="F41">
-        <v>9.25</v>
+        <v>121.01</v>
       </c>
       <c r="H41">
         <v>17</v>
       </c>
       <c r="I41">
-        <v>1940.93</v>
+        <v>4.9705399999999997E-2</v>
       </c>
       <c r="J41">
-        <v>762.31100000000004</v>
+        <v>4.8449800000000001E-2</v>
       </c>
       <c r="K41">
-        <v>21.491800000000001</v>
+        <v>5.2101799999999997E-2</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
@@ -6744,28 +6744,28 @@
         <v>100</v>
       </c>
       <c r="C42">
-        <v>206.76</v>
+        <v>0.40111200000000002</v>
       </c>
       <c r="D42">
-        <v>210</v>
+        <v>0.91107199999999999</v>
       </c>
       <c r="E42">
-        <v>7.5964799999999997</v>
+        <v>5.2831500000000003E-2</v>
       </c>
       <c r="F42">
-        <v>10.06</v>
+        <v>119.22</v>
       </c>
       <c r="H42">
         <v>18</v>
       </c>
       <c r="I42">
-        <v>1744.53</v>
+        <v>4.2482100000000002E-2</v>
       </c>
       <c r="J42">
-        <v>751.30200000000002</v>
+        <v>5.3605699999999999E-2</v>
       </c>
       <c r="K42">
-        <v>20.912099999999999</v>
+        <v>4.6669500000000003E-2</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
@@ -6776,28 +6776,28 @@
         <v>100</v>
       </c>
       <c r="C43">
-        <v>205.98500000000001</v>
+        <v>0.38604100000000002</v>
       </c>
       <c r="D43">
-        <v>210</v>
+        <v>1.00814</v>
       </c>
       <c r="E43">
-        <v>13.7227</v>
+        <v>5.1303799999999997E-2</v>
       </c>
       <c r="F43">
-        <v>11.21</v>
+        <v>131.32</v>
       </c>
       <c r="H43">
         <v>19</v>
       </c>
       <c r="I43">
-        <v>1820.5</v>
+        <v>4.4146499999999998E-2</v>
       </c>
       <c r="J43">
-        <v>756.82500000000005</v>
+        <v>5.21673E-2</v>
       </c>
       <c r="K43">
-        <v>17.221</v>
+        <v>5.9023100000000002E-2</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
@@ -6808,16 +6808,16 @@
         <v>100</v>
       </c>
       <c r="C44">
-        <v>205.56899999999999</v>
+        <v>0.371751</v>
       </c>
       <c r="D44">
-        <v>210</v>
+        <v>0.88690899999999995</v>
       </c>
       <c r="E44">
-        <v>14.6547</v>
+        <v>5.2113800000000002E-2</v>
       </c>
       <c r="F44">
-        <v>11.45</v>
+        <v>122.46</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
@@ -6828,16 +6828,16 @@
         <v>100</v>
       </c>
       <c r="C45">
-        <v>205.208</v>
+        <v>0.39919300000000002</v>
       </c>
       <c r="D45">
-        <v>210</v>
+        <v>0.79801999999999995</v>
       </c>
       <c r="E45">
-        <v>10.7919</v>
+        <v>4.6865400000000002E-2</v>
       </c>
       <c r="F45">
-        <v>12.06</v>
+        <v>128.06</v>
       </c>
       <c r="H45" t="s">
         <v>0</v>
@@ -6860,28 +6860,28 @@
         <v>100</v>
       </c>
       <c r="C46">
-        <v>204.607</v>
+        <v>0.36396699999999998</v>
       </c>
       <c r="D46">
-        <v>210</v>
+        <v>0.85635300000000003</v>
       </c>
       <c r="E46">
-        <v>17.158799999999999</v>
+        <v>4.7343200000000002E-2</v>
       </c>
       <c r="F46">
-        <v>12</v>
+        <v>120.69</v>
       </c>
       <c r="H46">
         <v>1</v>
       </c>
       <c r="I46">
-        <v>0.12</v>
+        <v>1.28</v>
       </c>
       <c r="J46">
-        <v>0.92</v>
+        <v>12.16</v>
       </c>
       <c r="K46">
-        <v>8.3800000000000008</v>
+        <v>117.49</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
@@ -6892,28 +6892,28 @@
         <v>100</v>
       </c>
       <c r="C47">
-        <v>204.1</v>
+        <v>0.36971500000000002</v>
       </c>
       <c r="D47">
-        <v>210</v>
+        <v>0.83546299999999996</v>
       </c>
       <c r="E47">
-        <v>18.426200000000001</v>
+        <v>4.4137999999999997E-2</v>
       </c>
       <c r="F47">
-        <v>12.18</v>
+        <v>126.72</v>
       </c>
       <c r="H47">
         <v>2</v>
       </c>
       <c r="I47">
-        <v>0.14000000000000001</v>
+        <v>1.3</v>
       </c>
       <c r="J47">
-        <v>0.95</v>
+        <v>11.95</v>
       </c>
       <c r="K47">
-        <v>9.25</v>
+        <v>121.01</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
@@ -6924,28 +6924,28 @@
         <v>100</v>
       </c>
       <c r="C48">
-        <v>204.197</v>
+        <v>0.37907000000000002</v>
       </c>
       <c r="D48">
-        <v>210</v>
+        <v>0.84770199999999996</v>
       </c>
       <c r="E48">
-        <v>14.172499999999999</v>
+        <v>4.5892299999999997E-2</v>
       </c>
       <c r="F48">
-        <v>12.89</v>
+        <v>120.54</v>
       </c>
       <c r="H48">
         <v>3</v>
       </c>
       <c r="I48">
-        <v>0.12</v>
+        <v>1.22</v>
       </c>
       <c r="J48">
-        <v>1</v>
+        <v>12.16</v>
       </c>
       <c r="K48">
-        <v>10.06</v>
+        <v>119.22</v>
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
@@ -6956,28 +6956,28 @@
         <v>100</v>
       </c>
       <c r="C49">
-        <v>204.58</v>
+        <v>0.33645900000000001</v>
       </c>
       <c r="D49">
-        <v>210</v>
+        <v>0.88817999999999997</v>
       </c>
       <c r="E49">
-        <v>14.708399999999999</v>
+        <v>5.0840999999999997E-2</v>
       </c>
       <c r="F49">
-        <v>13.48</v>
+        <v>117.75</v>
       </c>
       <c r="H49">
         <v>4</v>
       </c>
       <c r="I49">
-        <v>0.12</v>
+        <v>1.25</v>
       </c>
       <c r="J49">
-        <v>0.91</v>
+        <v>12.09</v>
       </c>
       <c r="K49">
-        <v>11.21</v>
+        <v>131.32</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
@@ -6988,28 +6988,28 @@
         <v>100</v>
       </c>
       <c r="C50">
-        <v>203.90299999999999</v>
+        <v>0.389544</v>
       </c>
       <c r="D50">
-        <v>209.83199999999999</v>
+        <v>0.96202799999999999</v>
       </c>
       <c r="E50">
-        <v>22.7133</v>
+        <v>4.8796300000000001E-2</v>
       </c>
       <c r="F50">
-        <v>13.51</v>
+        <v>115.6</v>
       </c>
       <c r="H50">
         <v>5</v>
       </c>
       <c r="I50">
-        <v>0.11</v>
+        <v>1.22</v>
       </c>
       <c r="J50">
-        <v>1.06</v>
+        <v>12.15</v>
       </c>
       <c r="K50">
-        <v>11.45</v>
+        <v>122.46</v>
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
@@ -7020,28 +7020,28 @@
         <v>100</v>
       </c>
       <c r="C51">
-        <v>203.09399999999999</v>
+        <v>0.41201199999999999</v>
       </c>
       <c r="D51">
-        <v>210</v>
+        <v>0.84602900000000003</v>
       </c>
       <c r="E51">
-        <v>22.4863</v>
+        <v>4.8807900000000001E-2</v>
       </c>
       <c r="F51">
-        <v>13.37</v>
+        <v>118.07</v>
       </c>
       <c r="H51">
         <v>6</v>
       </c>
       <c r="I51">
-        <v>7.0000000000000007E-2</v>
+        <v>1.28</v>
       </c>
       <c r="J51">
-        <v>1.06</v>
+        <v>12.03</v>
       </c>
       <c r="K51">
-        <v>12.06</v>
+        <v>128.06</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
@@ -7052,28 +7052,28 @@
         <v>100</v>
       </c>
       <c r="C52">
-        <v>203.09100000000001</v>
+        <v>0.375496</v>
       </c>
       <c r="D52">
-        <v>210</v>
+        <v>0.86468599999999995</v>
       </c>
       <c r="E52">
-        <v>17.845199999999998</v>
+        <v>4.4103000000000003E-2</v>
       </c>
       <c r="F52">
-        <v>14.41</v>
+        <v>117.65</v>
       </c>
       <c r="H52">
         <v>7</v>
       </c>
       <c r="I52">
-        <v>0.1</v>
+        <v>1.21</v>
       </c>
       <c r="J52">
-        <v>1.02</v>
+        <v>12.2</v>
       </c>
       <c r="K52">
-        <v>12</v>
+        <v>120.69</v>
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
@@ -7084,28 +7084,28 @@
         <v>100</v>
       </c>
       <c r="C53">
-        <v>202.91</v>
+        <v>0.39245400000000003</v>
       </c>
       <c r="D53">
-        <v>210</v>
+        <v>0.88642900000000002</v>
       </c>
       <c r="E53">
-        <v>28.591200000000001</v>
+        <v>5.5421900000000003E-2</v>
       </c>
       <c r="F53">
-        <v>15.09</v>
+        <v>121.25</v>
       </c>
       <c r="H53">
         <v>8</v>
       </c>
       <c r="I53">
-        <v>0.13</v>
+        <v>1.32</v>
       </c>
       <c r="J53">
-        <v>1.01</v>
+        <v>12.01</v>
       </c>
       <c r="K53">
-        <v>12.18</v>
+        <v>126.72</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
@@ -7116,28 +7116,28 @@
         <v>100</v>
       </c>
       <c r="C54">
-        <v>202.56800000000001</v>
+        <v>0.41637600000000002</v>
       </c>
       <c r="D54">
-        <v>209.90799999999999</v>
+        <v>0.863537</v>
       </c>
       <c r="E54">
-        <v>21.029699999999998</v>
+        <v>4.8130100000000002E-2</v>
       </c>
       <c r="F54">
-        <v>14.26</v>
+        <v>125.99</v>
       </c>
       <c r="H54">
         <v>9</v>
       </c>
       <c r="I54">
-        <v>0.1</v>
+        <v>1.22</v>
       </c>
       <c r="J54">
-        <v>1.1399999999999999</v>
+        <v>12.02</v>
       </c>
       <c r="K54">
-        <v>12.89</v>
+        <v>120.54</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
@@ -7148,28 +7148,28 @@
         <v>100</v>
       </c>
       <c r="C55">
-        <v>202.738</v>
+        <v>0.43040699999999998</v>
       </c>
       <c r="D55">
-        <v>210</v>
+        <v>0.93751799999999996</v>
       </c>
       <c r="E55">
-        <v>18.682300000000001</v>
+        <v>4.9035799999999997E-2</v>
       </c>
       <c r="F55">
-        <v>14.52</v>
+        <v>118.95</v>
       </c>
       <c r="H55">
         <v>10</v>
       </c>
       <c r="I55">
-        <v>0.1</v>
+        <v>1.25</v>
       </c>
       <c r="J55">
-        <v>1.06</v>
+        <v>11.8</v>
       </c>
       <c r="K55">
-        <v>13.48</v>
+        <v>117.75</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
@@ -7180,28 +7180,28 @@
         <v>100</v>
       </c>
       <c r="C56">
-        <v>201.73500000000001</v>
+        <v>0.37239899999999998</v>
       </c>
       <c r="D56">
-        <v>209.49199999999999</v>
+        <v>0.86468599999999995</v>
       </c>
       <c r="E56">
-        <v>21.491800000000001</v>
+        <v>5.2101799999999997E-2</v>
       </c>
       <c r="F56">
-        <v>15.02</v>
+        <v>118.51</v>
       </c>
       <c r="H56">
         <v>11</v>
       </c>
       <c r="I56">
-        <v>0.1</v>
+        <v>1.22</v>
       </c>
       <c r="J56">
-        <v>1.08</v>
+        <v>11.81</v>
       </c>
       <c r="K56">
-        <v>13.51</v>
+        <v>115.6</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
@@ -7212,28 +7212,28 @@
         <v>100</v>
       </c>
       <c r="C57">
-        <v>202.08600000000001</v>
+        <v>0.38234699999999999</v>
       </c>
       <c r="D57">
-        <v>210</v>
+        <v>0.92975300000000005</v>
       </c>
       <c r="E57">
-        <v>20.912099999999999</v>
+        <v>4.6669500000000003E-2</v>
       </c>
       <c r="F57">
-        <v>15.1</v>
+        <v>118.67</v>
       </c>
       <c r="H57">
         <v>12</v>
       </c>
       <c r="I57">
-        <v>0.11</v>
+        <v>1.22</v>
       </c>
       <c r="J57">
-        <v>1.04</v>
+        <v>11.75</v>
       </c>
       <c r="K57">
-        <v>13.37</v>
+        <v>118.07</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
@@ -7244,28 +7244,28 @@
         <v>100</v>
       </c>
       <c r="C58">
-        <v>202.42099999999999</v>
+        <v>0.408746</v>
       </c>
       <c r="D58">
-        <v>209.76900000000001</v>
+        <v>0.94246399999999997</v>
       </c>
       <c r="E58">
-        <v>17.221</v>
+        <v>5.9023100000000002E-2</v>
       </c>
       <c r="F58">
-        <v>16.14</v>
+        <v>120.58</v>
       </c>
       <c r="H58">
         <v>13</v>
       </c>
       <c r="I58">
-        <v>0.11</v>
+        <v>1.18</v>
       </c>
       <c r="J58">
-        <v>1.08</v>
+        <v>11.94</v>
       </c>
       <c r="K58">
-        <v>14.41</v>
+        <v>117.65</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
@@ -7273,13 +7273,13 @@
         <v>14</v>
       </c>
       <c r="I59">
-        <v>0.1</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="J59">
-        <v>0.96</v>
+        <v>11.73</v>
       </c>
       <c r="K59">
-        <v>15.09</v>
+        <v>121.25</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
@@ -7287,13 +7287,13 @@
         <v>15</v>
       </c>
       <c r="I60">
-        <v>0.16</v>
+        <v>1.2</v>
       </c>
       <c r="J60">
-        <v>1</v>
+        <v>11.87</v>
       </c>
       <c r="K60">
-        <v>14.26</v>
+        <v>125.99</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
@@ -7301,13 +7301,13 @@
         <v>16</v>
       </c>
       <c r="I61">
-        <v>0.1</v>
+        <v>1.25</v>
       </c>
       <c r="J61">
-        <v>1.21</v>
+        <v>11.8</v>
       </c>
       <c r="K61">
-        <v>14.52</v>
+        <v>118.95</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
@@ -7315,13 +7315,13 @@
         <v>17</v>
       </c>
       <c r="I62">
-        <v>0.09</v>
+        <v>1.25</v>
       </c>
       <c r="J62">
-        <v>1.05</v>
+        <v>12.01</v>
       </c>
       <c r="K62">
-        <v>15.02</v>
+        <v>118.51</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
@@ -7329,13 +7329,13 @@
         <v>18</v>
       </c>
       <c r="I63">
-        <v>0.09</v>
+        <v>1.19</v>
       </c>
       <c r="J63">
-        <v>1.05</v>
+        <v>11.8</v>
       </c>
       <c r="K63">
-        <v>15.1</v>
+        <v>118.67</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
@@ -7343,13 +7343,13 @@
         <v>19</v>
       </c>
       <c r="I64">
-        <v>0.09</v>
+        <v>1.24</v>
       </c>
       <c r="J64">
-        <v>1.01</v>
+        <v>11.83</v>
       </c>
       <c r="K64">
-        <v>16.14</v>
+        <v>120.58</v>
       </c>
     </row>
     <row r="66" spans="8:11" x14ac:dyDescent="0.25">
@@ -7371,13 +7371,13 @@
         <v>1</v>
       </c>
       <c r="I67">
-        <v>190.81200000000001</v>
+        <v>0.989672</v>
       </c>
       <c r="J67">
-        <v>210</v>
+        <v>0.88341800000000004</v>
       </c>
       <c r="K67">
-        <v>210</v>
+        <v>0.96306000000000003</v>
       </c>
     </row>
     <row r="68" spans="8:11" x14ac:dyDescent="0.25">
@@ -7385,13 +7385,13 @@
         <v>2</v>
       </c>
       <c r="I68">
-        <v>203.92500000000001</v>
+        <v>0.97313700000000003</v>
       </c>
       <c r="J68">
-        <v>209.495</v>
+        <v>0.893258</v>
       </c>
       <c r="K68">
-        <v>210</v>
+        <v>0.86468599999999995</v>
       </c>
     </row>
     <row r="69" spans="8:11" x14ac:dyDescent="0.25">
@@ -7399,13 +7399,13 @@
         <v>3</v>
       </c>
       <c r="I69">
-        <v>196.65899999999999</v>
+        <v>0.98524199999999995</v>
       </c>
       <c r="J69">
-        <v>210</v>
+        <v>0.86526899999999995</v>
       </c>
       <c r="K69">
-        <v>210</v>
+        <v>0.91107199999999999</v>
       </c>
     </row>
     <row r="70" spans="8:11" x14ac:dyDescent="0.25">
@@ -7413,13 +7413,13 @@
         <v>4</v>
       </c>
       <c r="I70">
-        <v>209.93299999999999</v>
+        <v>0.920242</v>
       </c>
       <c r="J70">
-        <v>210</v>
+        <v>0.89802000000000004</v>
       </c>
       <c r="K70">
-        <v>210</v>
+        <v>1.00814</v>
       </c>
     </row>
     <row r="71" spans="8:11" x14ac:dyDescent="0.25">
@@ -7427,13 +7427,13 @@
         <v>5</v>
       </c>
       <c r="I71">
-        <v>194.364</v>
+        <v>0.85992500000000005</v>
       </c>
       <c r="J71">
-        <v>210</v>
+        <v>0.81761200000000001</v>
       </c>
       <c r="K71">
-        <v>210</v>
+        <v>0.88690899999999995</v>
       </c>
     </row>
     <row r="72" spans="8:11" x14ac:dyDescent="0.25">
@@ -7441,13 +7441,13 @@
         <v>6</v>
       </c>
       <c r="I72">
-        <v>203.06</v>
+        <v>0.94246399999999997</v>
       </c>
       <c r="J72">
-        <v>210</v>
+        <v>0.88135300000000005</v>
       </c>
       <c r="K72">
-        <v>210</v>
+        <v>0.79801999999999995</v>
       </c>
     </row>
     <row r="73" spans="8:11" x14ac:dyDescent="0.25">
@@ -7455,13 +7455,13 @@
         <v>7</v>
       </c>
       <c r="I73">
-        <v>198.32400000000001</v>
+        <v>0.86858900000000006</v>
       </c>
       <c r="J73">
-        <v>209.44900000000001</v>
+        <v>0.85633899999999996</v>
       </c>
       <c r="K73">
-        <v>210</v>
+        <v>0.85635300000000003</v>
       </c>
     </row>
     <row r="74" spans="8:11" x14ac:dyDescent="0.25">
@@ -7469,13 +7469,13 @@
         <v>8</v>
       </c>
       <c r="I74">
-        <v>201.98500000000001</v>
+        <v>0.83135300000000001</v>
       </c>
       <c r="J74">
-        <v>208.90899999999999</v>
+        <v>0.87933799999999995</v>
       </c>
       <c r="K74">
-        <v>210</v>
+        <v>0.83546299999999996</v>
       </c>
     </row>
     <row r="75" spans="8:11" x14ac:dyDescent="0.25">
@@ -7483,13 +7483,13 @@
         <v>9</v>
       </c>
       <c r="I75">
-        <v>206.55600000000001</v>
+        <v>0.89802000000000004</v>
       </c>
       <c r="J75">
-        <v>210</v>
+        <v>0.831036</v>
       </c>
       <c r="K75">
-        <v>210</v>
+        <v>0.84770199999999996</v>
       </c>
     </row>
     <row r="76" spans="8:11" x14ac:dyDescent="0.25">
@@ -7497,13 +7497,13 @@
         <v>10</v>
       </c>
       <c r="I76">
-        <v>205.56299999999999</v>
+        <v>0.91303400000000001</v>
       </c>
       <c r="J76">
-        <v>210</v>
+        <v>0.91913100000000003</v>
       </c>
       <c r="K76">
-        <v>210</v>
+        <v>0.88817999999999997</v>
       </c>
     </row>
     <row r="77" spans="8:11" x14ac:dyDescent="0.25">
@@ -7511,13 +7511,13 @@
         <v>11</v>
       </c>
       <c r="I77">
-        <v>193.90199999999999</v>
+        <v>0.88135300000000005</v>
       </c>
       <c r="J77">
-        <v>210</v>
+        <v>0.87936199999999998</v>
       </c>
       <c r="K77">
-        <v>209.83199999999999</v>
+        <v>0.96202799999999999</v>
       </c>
     </row>
     <row r="78" spans="8:11" x14ac:dyDescent="0.25">
@@ -7525,13 +7525,13 @@
         <v>12</v>
       </c>
       <c r="I78">
-        <v>205.88900000000001</v>
+        <v>0.87135300000000004</v>
       </c>
       <c r="J78">
-        <v>209.715</v>
+        <v>0.88135300000000005</v>
       </c>
       <c r="K78">
-        <v>210</v>
+        <v>0.84602900000000003</v>
       </c>
     </row>
     <row r="79" spans="8:11" x14ac:dyDescent="0.25">
@@ -7539,13 +7539,13 @@
         <v>13</v>
       </c>
       <c r="I79">
-        <v>200.03899999999999</v>
+        <v>0.84413099999999996</v>
       </c>
       <c r="J79">
-        <v>208.953</v>
+        <v>0.86996399999999996</v>
       </c>
       <c r="K79">
-        <v>210</v>
+        <v>0.86468599999999995</v>
       </c>
     </row>
     <row r="80" spans="8:11" x14ac:dyDescent="0.25">
@@ -7553,13 +7553,13 @@
         <v>14</v>
       </c>
       <c r="I80">
-        <v>196.82900000000001</v>
+        <v>0.86563900000000005</v>
       </c>
       <c r="J80">
-        <v>210</v>
+        <v>1.03135</v>
       </c>
       <c r="K80">
-        <v>210</v>
+        <v>0.88642900000000002</v>
       </c>
     </row>
     <row r="81" spans="8:11" x14ac:dyDescent="0.25">
@@ -7567,13 +7567,13 @@
         <v>15</v>
       </c>
       <c r="I81">
-        <v>188.30799999999999</v>
+        <v>0.893258</v>
       </c>
       <c r="J81">
-        <v>210</v>
+        <v>0.90226200000000001</v>
       </c>
       <c r="K81">
-        <v>209.90799999999999</v>
+        <v>0.863537</v>
       </c>
     </row>
     <row r="82" spans="8:11" x14ac:dyDescent="0.25">
@@ -7581,13 +7581,13 @@
         <v>16</v>
       </c>
       <c r="I82">
-        <v>192.05199999999999</v>
+        <v>0.86468599999999995</v>
       </c>
       <c r="J82">
-        <v>209.22900000000001</v>
+        <v>0.81824399999999997</v>
       </c>
       <c r="K82">
-        <v>210</v>
+        <v>0.93751799999999996</v>
       </c>
     </row>
     <row r="83" spans="8:11" x14ac:dyDescent="0.25">
@@ -7595,13 +7595,13 @@
         <v>17</v>
       </c>
       <c r="I83">
-        <v>197.791</v>
+        <v>0.85194899999999996</v>
       </c>
       <c r="J83">
-        <v>210</v>
+        <v>0.83730599999999999</v>
       </c>
       <c r="K83">
-        <v>209.49199999999999</v>
+        <v>0.86468599999999995</v>
       </c>
     </row>
     <row r="84" spans="8:11" x14ac:dyDescent="0.25">
@@ -7609,13 +7609,13 @@
         <v>18</v>
       </c>
       <c r="I84">
-        <v>207.36</v>
+        <v>0.93135299999999999</v>
       </c>
       <c r="J84">
-        <v>209.65899999999999</v>
+        <v>0.95867500000000005</v>
       </c>
       <c r="K84">
-        <v>210</v>
+        <v>0.92975300000000005</v>
       </c>
     </row>
     <row r="85" spans="8:11" x14ac:dyDescent="0.25">
@@ -7623,13 +7623,13 @@
         <v>19</v>
       </c>
       <c r="I85">
-        <v>199.208</v>
+        <v>0.85992500000000005</v>
       </c>
       <c r="J85">
-        <v>209.828</v>
+        <v>1.01267</v>
       </c>
       <c r="K85">
-        <v>209.76900000000001</v>
+        <v>0.94246399999999997</v>
       </c>
     </row>
   </sheetData>

</xml_diff>